<commit_message>
Adding the latest code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KRISHNENTHU\IdeaProjects\seleniumbasics\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BB4CC7-01DE-444F-8585-60A74EB7E03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2811A84-B963-4AD4-B2BB-C360DA08474F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
     <sheet name="HomePage" sheetId="2" r:id="rId2"/>
+    <sheet name="RegistrationPage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Alfreds Futterkiste</t>
   </si>
@@ -86,6 +87,33 @@
   </si>
   <si>
     <t>Demo Web Shop</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm password</t>
+  </si>
+  <si>
+    <t>test123</t>
   </si>
 </sst>
 </file>
@@ -492,7 +520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D9A01E-96FF-41C6-BE7B-EE6F262FBB05}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -513,4 +541,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD9899F-3965-406B-9CF6-650D0BDEF087}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>